<commit_message>
Will erase most blob detection settings to minimize the error
</commit_message>
<xml_diff>
--- a/Image processing comparison/negatives.xlsx
+++ b/Image processing comparison/negatives.xlsx
@@ -453,7 +453,7 @@
         <v>9</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>5.077576160430908</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -493,7 +493,7 @@
         <v>9</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>3.634586334228516</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -513,7 +513,7 @@
         <v>9</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>3.613167524337769</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -533,7 +533,7 @@
         <v>10</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>2.955438852310181</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -593,7 +593,7 @@
         <v>10</v>
       </c>
       <c r="C9">
-        <v>6.934174537658691</v>
+        <v>7.289011478424072</v>
       </c>
       <c r="D9">
         <v>9.233729362487793</v>
@@ -613,7 +613,7 @@
         <v>11</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>2.955438852310181</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -633,7 +633,7 @@
         <v>11</v>
       </c>
       <c r="C11">
-        <v>9.254150390625</v>
+        <v>9.361291885375977</v>
       </c>
       <c r="D11">
         <v>8.06851863861084</v>
@@ -653,7 +653,7 @@
         <v>11</v>
       </c>
       <c r="C12">
-        <v>6.709136009216309</v>
+        <v>10.91279149055481</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -673,7 +673,7 @@
         <v>11</v>
       </c>
       <c r="C13">
-        <v>15.63311672210693</v>
+        <v>16.16635513305664</v>
       </c>
       <c r="D13">
         <v>9.055385589599609</v>
@@ -693,7 +693,7 @@
         <v>12</v>
       </c>
       <c r="C14">
-        <v>6.210140705108643</v>
+        <v>8.831316709518433</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -733,7 +733,7 @@
         <v>12</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>4.448910713195801</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -753,7 +753,7 @@
         <v>12</v>
       </c>
       <c r="C17">
-        <v>8.05933666229248</v>
+        <v>11.33061385154724</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -773,7 +773,7 @@
         <v>13</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>2.955438852310181</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -813,7 +813,7 @@
         <v>13</v>
       </c>
       <c r="C20">
-        <v>8.027070045471191</v>
+        <v>7.917736530303955</v>
       </c>
       <c r="D20">
         <v>9.193733215332031</v>
@@ -833,7 +833,7 @@
         <v>13</v>
       </c>
       <c r="C21">
-        <v>5.296806812286377</v>
+        <v>14.84580516815186</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -853,7 +853,7 @@
         <v>14</v>
       </c>
       <c r="C22">
-        <v>5.073776245117188</v>
+        <v>22.16390085220337</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -893,7 +893,7 @@
         <v>14</v>
       </c>
       <c r="C24">
-        <v>8.876328468322754</v>
+        <v>12.40105843544006</v>
       </c>
       <c r="D24">
         <v>8.954010009765625</v>
@@ -913,7 +913,7 @@
         <v>14</v>
       </c>
       <c r="C25">
-        <v>0</v>
+        <v>8.337146282196045</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -933,7 +933,7 @@
         <v>15</v>
       </c>
       <c r="C26">
-        <v>0</v>
+        <v>4.315976142883301</v>
       </c>
       <c r="D26">
         <v>0</v>
@@ -973,10 +973,10 @@
         <v>15</v>
       </c>
       <c r="C28">
-        <v>0</v>
+        <v>11.40879583358765</v>
       </c>
       <c r="D28">
-        <v>7.280109882354736</v>
+        <v>0</v>
       </c>
       <c r="E28">
         <v>8.123106002807617</v>
@@ -1053,7 +1053,7 @@
         <v>16</v>
       </c>
       <c r="C32">
-        <v>26.15472507476807</v>
+        <v>31.79722595214844</v>
       </c>
       <c r="D32">
         <v>28.52133655548096</v>

</xml_diff>